<commit_message>
New Version v3: - Incresed DC-DC converter max current to 500mA (saltuary brownout at boot) - Removed IO0 pull down capacitor (boot always in download mode) - New Level shiter circuits - Changed the LDO
</commit_message>
<xml_diff>
--- a/BOM_TSDZ2-ESP32.xlsx
+++ b/BOM_TSDZ2-ESP32.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Desktop\PCB\TSDz2-ESP32v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Massimo\Priv\Ebk\TSDZ2\BT\TSDZ2_ESP32\TSDZ2-ESP32-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9DB7D5B0-A936-467E-920F-8F1582CBDD7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5A7CFE-51AD-4686-9797-B75653B4CD92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="636" windowWidth="22260" windowHeight="11736"/>
+    <workbookView xWindow="216" yWindow="792" windowWidth="22128" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM_TSDZ2-ESP32-v2_202003092326" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM_TSDZ2-ESP32-v3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="166">
   <si>
     <t>ID</t>
   </si>
@@ -61,7 +61,7 @@
     <t>U1</t>
   </si>
   <si>
-    <t>VSON-10_L3.0-W3.0-P0.50-TL-EP</t>
+    <t>LM5166</t>
   </si>
   <si>
     <t>Texas Instruments</t>
@@ -79,307 +79,412 @@
     <t>Align dot on chip with dot on PCB (pin 1)</t>
   </si>
   <si>
-    <t>56.2K</t>
+    <t>309K</t>
+  </si>
+  <si>
+    <t>R2,R4</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>RC-02W3093FT</t>
+  </si>
+  <si>
+    <t>Guangdong Fenghua Advanced Tech</t>
+  </si>
+  <si>
+    <t>C321438</t>
+  </si>
+  <si>
+    <t>CHIP RES. 309K Ohm 1%  1/16W 0402</t>
+  </si>
+  <si>
+    <t>U.FL-R-SMT-1(80)</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>RF-SMD_U.FL-R-SMT-1(80)</t>
+  </si>
+  <si>
+    <t>HRS</t>
+  </si>
+  <si>
+    <t>C88374</t>
+  </si>
+  <si>
+    <t>RF Connectors 50Ohm U.FL</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>CL05B103KB5NNNC</t>
+  </si>
+  <si>
+    <t>SAMSUNG</t>
+  </si>
+  <si>
+    <t>C15195</t>
+  </si>
+  <si>
+    <t>CAP. CER. 10nF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>CL21B475KPFNNNE</t>
+  </si>
+  <si>
+    <t>C87998</t>
+  </si>
+  <si>
+    <t>CAP. CER. 4.7UF 10V X7R 0805</t>
+  </si>
+  <si>
+    <t>M74VHC1GT126DF1G</t>
+  </si>
+  <si>
+    <t>U6,U7</t>
+  </si>
+  <si>
+    <t>M74VHC1GT</t>
+  </si>
+  <si>
+    <t>ON Semicon</t>
+  </si>
+  <si>
+    <t>C150237</t>
+  </si>
+  <si>
+    <t>IC Noninverting Buffer SOT−353</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>R7,R6,R8,R10</t>
+  </si>
+  <si>
+    <t>RC-02W1002FT</t>
+  </si>
+  <si>
+    <t>C258091</t>
+  </si>
+  <si>
+    <t>CHIP RES. 10K Ohm 1%  1/16W 0402</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>0402WGF4701TCE</t>
+  </si>
+  <si>
+    <t>UniOhm</t>
+  </si>
+  <si>
+    <t>C25900</t>
+  </si>
+  <si>
+    <t>CHIP RES. 4.7K Ohm 1%  1/16W 0402</t>
+  </si>
+  <si>
+    <t>SN74LVC2G17DCKR</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>74LVC2G17</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>C50714</t>
+  </si>
+  <si>
+    <t>IC Dual Schmitt-Trigger Buffer SOT-363</t>
+  </si>
+  <si>
+    <t>CIN1</t>
+  </si>
+  <si>
+    <t>C1210</t>
+  </si>
+  <si>
+    <t>HMK325C7475KMHPE</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>C385986</t>
+  </si>
+  <si>
+    <t>CAP. CER. 4.7UF 100V X7S 1210</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>WR06X105 JTL</t>
+  </si>
+  <si>
+    <t>Walsin Tech Corp</t>
+  </si>
+  <si>
+    <t>C384292</t>
+  </si>
+  <si>
+    <t>CHIP RES. 1M Ohm 5%  1/10W 0603</t>
+  </si>
+  <si>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>GRM32ER71A476KE15L</t>
+  </si>
+  <si>
+    <t>MuRata</t>
+  </si>
+  <si>
+    <t>C84494</t>
+  </si>
+  <si>
+    <t>CAP. CER. 47UF 10V X7R 1210</t>
+  </si>
+  <si>
+    <t>1.25T-1-4A</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>BOOMELE</t>
+  </si>
+  <si>
+    <t>C10821</t>
+  </si>
+  <si>
+    <t>Wire to Board connector male T.H. 1.25mm 4 pos.</t>
+  </si>
+  <si>
+    <t>XH-3A</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>CONN-TH_XH-3A</t>
+  </si>
+  <si>
+    <t>C2316</t>
+  </si>
+  <si>
+    <t>Wire to Board connector, male, T.H., XH 2.5mm, 3 pos.</t>
+  </si>
+  <si>
+    <t>100pF</t>
+  </si>
+  <si>
+    <t>CFF</t>
+  </si>
+  <si>
+    <t>C0402C101K5RACAUTO</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C141051</t>
+  </si>
+  <si>
+    <t>CAP. CER. 100pF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>1.25T-1-3A</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>C10820</t>
+  </si>
+  <si>
+    <t>Wire to Board connector male T.H. 1.25mm 3 pos.</t>
+  </si>
+  <si>
+    <t>Header-Male-2.54_2x4</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>HDR-TH_8P-P2.54-V-R2-C4-S2.54</t>
+  </si>
+  <si>
+    <t>210S-2*4P L=11.6MMGold-plated black</t>
+  </si>
+  <si>
+    <t>Ckmtw</t>
+  </si>
+  <si>
+    <t>C124386</t>
+  </si>
+  <si>
+    <t>Pin Header Male, 2.54mm, 2x4</t>
+  </si>
+  <si>
+    <t>TPS73533DRVR</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>QFN-6_L2.0-W2.0-P0.65-BL-EP</t>
+  </si>
+  <si>
+    <t>C48984</t>
+  </si>
+  <si>
+    <t>IC LDO 3.3V 500mA SON-6</t>
+  </si>
+  <si>
+    <t>MBR130T1G</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SOD-123_L2.8-W1.8-LS3.7-RD</t>
+  </si>
+  <si>
+    <t>C82461</t>
+  </si>
+  <si>
+    <t>Schottky Barrier Diode 30V, 470mV@1A, SOD-123</t>
+  </si>
+  <si>
+    <t>0.12</t>
   </si>
   <si>
     <t>R1</t>
   </si>
   <si>
-    <t>R0402</t>
-  </si>
-  <si>
-    <t>0402WGF5622TCE</t>
-  </si>
-  <si>
-    <t>UniOhm</t>
-  </si>
-  <si>
-    <t>C54968</t>
-  </si>
-  <si>
-    <t>CHIP RES. 56.2K Ohm 1%  1/16W 0402</t>
-  </si>
-  <si>
-    <t>309K</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>RC-02W3093FT</t>
-  </si>
-  <si>
-    <t>Guangdong Fenghua Advanced Tech</t>
-  </si>
-  <si>
-    <t>C321438</t>
-  </si>
-  <si>
-    <t>CHIP RES. 309K Ohm 1%  1/16W 0402</t>
-  </si>
-  <si>
-    <t>U.FL-R-SMT-1(80)</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>RF-SMD_U.FL-R-SMT-1(80)</t>
-  </si>
-  <si>
-    <t>HRS</t>
-  </si>
-  <si>
-    <t>C88374</t>
-  </si>
-  <si>
-    <t>RF Connectors 50Ohm U.FL</t>
-  </si>
-  <si>
-    <t>22uH</t>
+    <t>0603WAF120LT5E</t>
+  </si>
+  <si>
+    <t>Uniroyal Elec</t>
+  </si>
+  <si>
+    <t>C247139</t>
+  </si>
+  <si>
+    <t>CHIP RES. 0.12 Ohm 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>C8,C7,C6,C5,C11,C10,C9</t>
+  </si>
+  <si>
+    <t>0402'</t>
+  </si>
+  <si>
+    <t>GCM155R71C104KA40D</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>C126523</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>R12,R11</t>
+  </si>
+  <si>
+    <t>RC0402FR-07360RL</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>C138000</t>
+  </si>
+  <si>
+    <t>CHIP RES. 360 Ohm 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>TMP112AIDRLR</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>TMP112A</t>
+  </si>
+  <si>
+    <t>C28927</t>
+  </si>
+  <si>
+    <t>IC Temp. Sensor SOT563</t>
+  </si>
+  <si>
+    <t>Align pin 1 with dot on PCB (pin 1)</t>
+  </si>
+  <si>
+    <t>180uH</t>
   </si>
   <si>
     <t>L1</t>
   </si>
   <si>
-    <t>IND-SMD_L5.0-W5.0-P3.60_SMNR5040</t>
-  </si>
-  <si>
-    <t>SMNR5040-220MT</t>
-  </si>
-  <si>
-    <t>SXN</t>
-  </si>
-  <si>
-    <t>C9391</t>
-  </si>
-  <si>
-    <t>Power Inductor 22uH ±20% 1.4A SMD,5.0x5.0x4.0mm</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C0402</t>
-  </si>
-  <si>
-    <t>CL05B103KB5NNNC</t>
-  </si>
-  <si>
-    <t>SAMSUNG</t>
-  </si>
-  <si>
-    <t>C15195</t>
-  </si>
-  <si>
-    <t>CAP. CER. 10nF 25V X7R 0402</t>
-  </si>
-  <si>
-    <t>4.7K</t>
-  </si>
-  <si>
-    <t>R3,R6,R7</t>
-  </si>
-  <si>
-    <t>CR0402JF0472G</t>
-  </si>
-  <si>
-    <t>LIZ</t>
-  </si>
-  <si>
-    <t>C100658</t>
-  </si>
-  <si>
-    <t>CHIP RES. 4.7K Ohm 5%  1/16W 0402</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C0603</t>
-  </si>
-  <si>
-    <t>CL10B105KA8NNNC</t>
-  </si>
-  <si>
-    <t>C29936</t>
-  </si>
-  <si>
-    <t>CAP. CER. 1UF 25V X7R 0603</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>0603B225K160NT</t>
-  </si>
-  <si>
-    <t>FH</t>
-  </si>
-  <si>
-    <t>C43922</t>
-  </si>
-  <si>
-    <t>CAP. CER. 2.2UF 25V X7R 0603</t>
-  </si>
-  <si>
-    <t>47uF</t>
-  </si>
-  <si>
-    <t>CO2,CO1</t>
-  </si>
-  <si>
-    <t>C1210</t>
-  </si>
-  <si>
-    <t>GRM32ER71A476KE15L</t>
-  </si>
-  <si>
-    <t>MuRata</t>
-  </si>
-  <si>
-    <t>C84494</t>
-  </si>
-  <si>
-    <t>CAP CER 47UF 10V X7R 1210</t>
-  </si>
-  <si>
-    <t>TXS0104ERGYR</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>VQFN-14_L3.5-W3.5-P0.50-BL-EP</t>
-  </si>
-  <si>
-    <t>C154926</t>
-  </si>
-  <si>
-    <t>IC Level Translators VQFN-14_3.6x3.6x05P</t>
-  </si>
-  <si>
-    <t>220nF</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C1206</t>
-  </si>
-  <si>
-    <t>GCJ31MR72A224KA01L</t>
-  </si>
-  <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
-    <t>C363946</t>
-  </si>
-  <si>
-    <t>CAP CER 220nF 100V X7R 1206</t>
-  </si>
-  <si>
-    <t>NCV8535MN330R2G</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>NCV8535</t>
-  </si>
-  <si>
-    <t>ON Semicon</t>
-  </si>
-  <si>
-    <t>C114799</t>
-  </si>
-  <si>
-    <t>IC LDO 3.3V 500mA Reverse Voltage protection DFN-10_EP_3x3mm</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>C4,C3,C5,C6,C7,C9,C8</t>
-  </si>
-  <si>
-    <t>0402'</t>
-  </si>
-  <si>
-    <t>GCM155R71C104KA40D</t>
-  </si>
-  <si>
-    <t>C126523</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 10V X7R 0402</t>
-  </si>
-  <si>
-    <t>TMP112AIDRLR</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-563_L1.6-W1.2-P0.50-LS1.6-BL</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>C28927</t>
-  </si>
-  <si>
-    <t>IC Temp. Sensor SOT563</t>
-  </si>
-  <si>
-    <t>Align pin 1 with dot on PCB (pin 1)</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>HQ02WAJ0103TCE</t>
-  </si>
-  <si>
-    <t>UNI-ROYAL(Uniroyal Elec)</t>
-  </si>
-  <si>
-    <t>C414854</t>
-  </si>
-  <si>
-    <t>CHIP RES. 10K Ohm 5%  1/16W 0402</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>CIN</t>
-  </si>
-  <si>
-    <t>C1210X475K101T</t>
-  </si>
-  <si>
-    <t>Holy Stone Enterprise</t>
-  </si>
-  <si>
-    <t>C337978</t>
-  </si>
-  <si>
-    <t>CAP CER 4.7UF 100V X7R 1210</t>
+    <t>IND-SMD_L10.5-W10.5</t>
+  </si>
+  <si>
+    <t>SCDS105R-181M-N</t>
+  </si>
+  <si>
+    <t>Chilisin Elec</t>
+  </si>
+  <si>
+    <t>C329730</t>
+  </si>
+  <si>
+    <t>Power Inductor 180uH ±20% 1.04A SMD,10.5x10.3.0mm</t>
   </si>
   <si>
     <t>ESP32-PICO-D4</t>
@@ -388,7 +493,7 @@
     <t>U3</t>
   </si>
   <si>
-    <t>QFN-48_L7.0-W7.0-P0.50-TL-EP5.1</t>
+    <t>ESP32-PICO-D4-H</t>
   </si>
   <si>
     <t>Espressif Systems</t>
@@ -403,7 +508,7 @@
     <t>100K</t>
   </si>
   <si>
-    <t>R5</t>
+    <t>R3,R13</t>
   </si>
   <si>
     <t>RC-02W1003FT</t>
@@ -413,30 +518,12 @@
   </si>
   <si>
     <t>CHIP RES. 100K Ohm 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>RIN</t>
-  </si>
-  <si>
-    <t>R1210</t>
-  </si>
-  <si>
-    <t>1210W2J0270T5E</t>
-  </si>
-  <si>
-    <t>C396488</t>
-  </si>
-  <si>
-    <t>CHIP RES. 27 Ohm 5% 1/2W 1210</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1270,26 +1357,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="57.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1376,7 +1464,7 @@
         <v>21</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>22</v>
@@ -1405,13 +1493,13 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -1443,19 +1531,19 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1463,22 +1551,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -1504,22 +1592,25 @@
         <v>47</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>50</v>
       </c>
-      <c r="J7" t="s">
-        <v>51</v>
+      <c r="K7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1527,31 +1618,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
         <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
         <v>54</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
         <v>55</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1559,31 +1650,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
         <v>61</v>
-      </c>
-      <c r="G9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1591,31 +1682,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
         <v>66</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>67</v>
       </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" t="s">
-        <v>69</v>
+      <c r="K10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1623,31 +1717,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
         <v>70</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G11" t="s">
         <v>71</v>
       </c>
-      <c r="D11" t="s">
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
         <v>72</v>
       </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="J11" t="s">
         <v>73</v>
-      </c>
-      <c r="G11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s">
-        <v>75</v>
-      </c>
-      <c r="J11" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1655,13 +1749,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1670,19 +1764,16 @@
         <v>77</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
       </c>
       <c r="I12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" t="s">
         <v>80</v>
-      </c>
-      <c r="J12" t="s">
-        <v>81</v>
-      </c>
-      <c r="K12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1690,31 +1781,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
         <v>82</v>
       </c>
-      <c r="C13" t="s">
-        <v>83</v>
-      </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
         <v>85</v>
       </c>
-      <c r="G13" t="s">
+      <c r="J13" t="s">
         <v>86</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J13" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1722,34 +1813,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" t="s">
         <v>89</v>
       </c>
-      <c r="G14" t="s">
-        <v>92</v>
-      </c>
       <c r="H14" t="s">
         <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J14" t="s">
-        <v>94</v>
-      </c>
-      <c r="K14" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1757,31 +1845,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
         <v>95</v>
       </c>
-      <c r="C15" t="s">
+      <c r="J15" t="s">
         <v>96</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15">
-        <v>7</v>
-      </c>
-      <c r="F15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>99</v>
-      </c>
-      <c r="J15" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1789,34 +1877,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
         <v>101</v>
       </c>
-      <c r="G16" t="s">
-        <v>104</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>105</v>
-      </c>
       <c r="J16" t="s">
-        <v>106</v>
-      </c>
-      <c r="K16" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1824,31 +1909,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G17" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="J17" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1856,31 +1941,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J18" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1888,31 +1973,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G19" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="J19" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -1923,31 +2008,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G20" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="J20" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1955,31 +2040,229 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>128</v>
+      </c>
+      <c r="J21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" t="s">
         <v>134</v>
       </c>
-      <c r="G21" t="s">
-        <v>111</v>
-      </c>
-      <c r="H21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
         <v>135</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J22" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>360</v>
+      </c>
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>140</v>
+      </c>
+      <c r="J23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>145</v>
+      </c>
+      <c r="J24" t="s">
+        <v>146</v>
+      </c>
+      <c r="K24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>151</v>
+      </c>
+      <c r="G25" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
+        <v>153</v>
+      </c>
+      <c r="J25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" t="s">
+        <v>157</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" t="s">
+        <v>158</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s">
+        <v>159</v>
+      </c>
+      <c r="J26" t="s">
+        <v>160</v>
+      </c>
+      <c r="K26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" t="s">
+        <v>162</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>164</v>
+      </c>
+      <c r="J27" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM (all components in stock on LCSC on 2/6/2020)
</commit_message>
<xml_diff>
--- a/BOM_TSDZ2-ESP32.xlsx
+++ b/BOM_TSDZ2-ESP32.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Massimo\Priv\Ebk\TSDZ2\BT\TSDZ2_ESP32\TSDZ2-ESP32-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5A7CFE-51AD-4686-9797-B75653B4CD92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A005FD-391D-4E50-AAF4-FD3BEFBD2FE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="216" yWindow="792" windowWidth="22128" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3792" yWindow="1176" windowWidth="19248" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_TSDZ2-ESP32-v3" sheetId="1" r:id="rId1"/>
@@ -88,15 +88,9 @@
     <t>R0402</t>
   </si>
   <si>
-    <t>RC-02W3093FT</t>
-  </si>
-  <si>
     <t>Guangdong Fenghua Advanced Tech</t>
   </si>
   <si>
-    <t>C321438</t>
-  </si>
-  <si>
     <t>CHIP RES. 309K Ohm 1%  1/16W 0402</t>
   </si>
   <si>
@@ -518,6 +512,12 @@
   </si>
   <si>
     <t>CHIP RES. 100K Ohm 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>WR04X3093FTL</t>
+  </si>
+  <si>
+    <t>C334683</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1361,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1467,19 +1467,19 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
       <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1487,31 +1487,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
         <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1519,31 +1519,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1551,31 +1551,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
         <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1583,31 +1583,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
         <v>48</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" t="s">
-        <v>50</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
@@ -1618,10 +1618,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1630,19 +1630,19 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" t="s">
         <v>53</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1650,10 +1650,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -1662,19 +1662,19 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
         <v>58</v>
       </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
         <v>59</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1682,31 +1682,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
         <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
         <v>65</v>
-      </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" t="s">
-        <v>67</v>
       </c>
       <c r="K10" t="s">
         <v>18</v>
@@ -1717,31 +1717,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
         <v>70</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
         <v>71</v>
-      </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1749,31 +1749,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
         <v>74</v>
-      </c>
-      <c r="C12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
         <v>77</v>
       </c>
-      <c r="G12" t="s">
+      <c r="J12" t="s">
         <v>78</v>
-      </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1781,31 +1781,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
         <v>83</v>
       </c>
-      <c r="G13" t="s">
+      <c r="J13" t="s">
         <v>84</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1813,31 +1813,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
         <v>87</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" t="s">
         <v>89</v>
-      </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1845,31 +1845,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
         <v>92</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" t="s">
-        <v>94</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
       </c>
       <c r="I15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1877,31 +1877,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
         <v>99</v>
       </c>
-      <c r="G16" t="s">
+      <c r="J16" t="s">
         <v>100</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>101</v>
-      </c>
-      <c r="J16" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1909,31 +1909,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
         <v>103</v>
       </c>
-      <c r="G17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" t="s">
-        <v>105</v>
-      </c>
       <c r="J17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1941,31 +1941,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
         <v>107</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" t="s">
-        <v>109</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
         <v>110</v>
       </c>
-      <c r="G18" t="s">
+      <c r="J18" t="s">
         <v>111</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" t="s">
-        <v>112</v>
-      </c>
-      <c r="J18" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1973,31 +1973,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" t="s">
         <v>114</v>
-      </c>
-      <c r="C19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" t="s">
-        <v>116</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -2008,31 +2008,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
         <v>119</v>
-      </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20" t="s">
-        <v>121</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2040,31 +2040,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
         <v>126</v>
       </c>
-      <c r="G21" t="s">
+      <c r="J21" t="s">
         <v>127</v>
-      </c>
-      <c r="H21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" t="s">
-        <v>128</v>
-      </c>
-      <c r="J21" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2072,31 +2072,31 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" t="s">
         <v>130</v>
-      </c>
-      <c r="C22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" t="s">
-        <v>132</v>
       </c>
       <c r="E22">
         <v>7</v>
       </c>
       <c r="F22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
         <v>133</v>
       </c>
-      <c r="G22" t="s">
+      <c r="J22" t="s">
         <v>134</v>
-      </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" t="s">
-        <v>135</v>
-      </c>
-      <c r="J22" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -2107,7 +2107,7 @@
         <v>360</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
@@ -2116,19 +2116,19 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
         <v>138</v>
       </c>
-      <c r="G23" t="s">
+      <c r="J23" t="s">
         <v>139</v>
-      </c>
-      <c r="H23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -2136,34 +2136,34 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" t="s">
         <v>142</v>
-      </c>
-      <c r="C24" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" t="s">
-        <v>144</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H24" t="s">
         <v>15</v>
       </c>
       <c r="I24" t="s">
+        <v>143</v>
+      </c>
+      <c r="J24" t="s">
+        <v>144</v>
+      </c>
+      <c r="K24" t="s">
         <v>145</v>
-      </c>
-      <c r="J24" t="s">
-        <v>146</v>
-      </c>
-      <c r="K24" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -2171,31 +2171,31 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" t="s">
         <v>148</v>
-      </c>
-      <c r="C25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" t="s">
-        <v>150</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" t="s">
+        <v>150</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
         <v>151</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>152</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" t="s">
-        <v>153</v>
-      </c>
-      <c r="J25" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -2203,31 +2203,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" t="s">
         <v>155</v>
-      </c>
-      <c r="C26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D26" t="s">
-        <v>157</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s">
+        <v>157</v>
+      </c>
+      <c r="J26" t="s">
         <v>158</v>
-      </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" t="s">
-        <v>159</v>
-      </c>
-      <c r="J26" t="s">
-        <v>160</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
@@ -2238,10 +2238,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
@@ -2250,19 +2250,19 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>162</v>
+      </c>
+      <c r="J27" t="s">
         <v>163</v>
-      </c>
-      <c r="G27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" t="s">
-        <v>164</v>
-      </c>
-      <c r="J27" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V4 Update: L1 Inductor from 47uF to 100uF (better low current regulation)
</commit_message>
<xml_diff>
--- a/BOM_TSDZ2-ESP32.xlsx
+++ b/BOM_TSDZ2-ESP32.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SO000228\Desktop\TSDZ2_ESP32_v4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SO000228\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5109F57-F7DF-4A6C-90E3-AE49C74EF20A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64550B13-9478-4FB1-A50C-2AC62EF8C723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="22872" windowHeight="11064" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1512" yWindow="912" windowWidth="21528" windowHeight="12048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PCB_2021-10-07" sheetId="1" r:id="rId1"/>
@@ -238,18 +238,9 @@
     <t>Sunlord</t>
   </si>
   <si>
-    <t>SWPA5040S470MT</t>
-  </si>
-  <si>
-    <t>INDUCTOR SMD 47uF 0.9A 5x5mm</t>
-  </si>
-  <si>
     <t>SMD_L5.0-W5.0</t>
   </si>
   <si>
-    <t>C86617</t>
-  </si>
-  <si>
     <t>U6,U5</t>
   </si>
   <si>
@@ -458,6 +449,15 @@
   </si>
   <si>
     <t>B-2100S06P-B110</t>
+  </si>
+  <si>
+    <t>SWPA5040S101MT</t>
+  </si>
+  <si>
+    <t>INDUCTOR SMD 100uF 0.75A 5x5mm</t>
+  </si>
+  <si>
+    <t>C88132</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1400,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1570,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -1811,19 +1811,19 @@
         <v>71</v>
       </c>
       <c r="E14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" t="s">
         <v>72</v>
       </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" t="s">
-        <v>74</v>
-      </c>
       <c r="H14" t="s">
         <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1831,28 +1831,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" t="s">
         <v>77</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
         <v>78</v>
-      </c>
-      <c r="F15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1860,28 +1860,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
         <v>83</v>
       </c>
-      <c r="E16" t="s">
+      <c r="H16" t="s">
         <v>84</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" t="s">
         <v>85</v>
-      </c>
-      <c r="G16" t="s">
-        <v>86</v>
-      </c>
-      <c r="H16" t="s">
-        <v>87</v>
-      </c>
-      <c r="I16" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1889,28 +1889,28 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" t="s">
         <v>90</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1918,28 +1918,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" t="s">
         <v>95</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1947,28 +1947,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" t="s">
         <v>100</v>
       </c>
-      <c r="E19" t="s">
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
         <v>101</v>
-      </c>
-      <c r="F19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1976,28 +1976,28 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" t="s">
         <v>106</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" t="s">
         <v>107</v>
-      </c>
-      <c r="F20" t="s">
-        <v>108</v>
-      </c>
-      <c r="G20" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -2005,28 +2005,28 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -2034,28 +2034,28 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" t="s">
         <v>116</v>
       </c>
-      <c r="E22" t="s">
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
         <v>117</v>
-      </c>
-      <c r="F22" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" t="s">
-        <v>119</v>
-      </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -2063,28 +2063,28 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" t="s">
         <v>77</v>
       </c>
-      <c r="E23" t="s">
-        <v>122</v>
-      </c>
-      <c r="F23" t="s">
-        <v>123</v>
-      </c>
-      <c r="G23" t="s">
-        <v>80</v>
-      </c>
       <c r="H23" t="s">
         <v>15</v>
       </c>
       <c r="I23" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -2092,28 +2092,28 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" t="s">
         <v>126</v>
       </c>
-      <c r="E24" t="s">
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
         <v>127</v>
-      </c>
-      <c r="F24" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" t="s">
-        <v>129</v>
-      </c>
-      <c r="H24" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -2121,28 +2121,28 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" t="s">
         <v>132</v>
       </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
         <v>133</v>
-      </c>
-      <c r="F25" t="s">
-        <v>134</v>
-      </c>
-      <c r="G25" t="s">
-        <v>135</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -2150,28 +2150,28 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s">
         <v>138</v>
-      </c>
-      <c r="E26" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>